<commit_message>
fix: Modify test units according to the changes in preprocessing for new merging.
</commit_message>
<xml_diff>
--- a/tests/data_test/GT_test.xlsx
+++ b/tests/data_test/GT_test.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilsonlozanor/Box/ResearchCUTR/data_OBA_loggers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilsonlozanor/PycharmProjects/onebusaway-travel-behavior-analysis/tests/data_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9AE98A-213E-D642-806A-8C8C3EC5D6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255138D6-0418-254B-AB99-55AAA675B0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36700" yWindow="-5520" windowWidth="31700" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -175,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -215,6 +226,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,8 +452,8 @@
   </sheetPr>
   <dimension ref="A1:X1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -444,7 +461,8 @@
     <col min="6" max="6" width="30" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" style="17"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -539,17 +557,23 @@
       <c r="K2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="32">
+        <f>F3</f>
+        <v>0.65406249999999999</v>
+      </c>
+      <c r="M2" s="31">
+        <v>0</v>
+      </c>
       <c r="N2" s="9">
         <v>42.617975999999999</v>
       </c>
       <c r="O2" s="9">
         <v>-92.312387999999999</v>
       </c>
-      <c r="P2" s="27" t="s">
+      <c r="P2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="28"/>
+      <c r="Q2" s="30"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -592,7 +616,13 @@
       <c r="K3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="28"/>
+      <c r="L3" s="32">
+        <f t="shared" ref="L3:L40" si="0">F4</f>
+        <v>0.6655092592592593</v>
+      </c>
+      <c r="M3" s="31">
+        <v>0</v>
+      </c>
       <c r="N3" s="9">
         <v>42.617718000000004</v>
       </c>
@@ -644,6 +674,13 @@
       <c r="K4" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="L4" s="32">
+        <f t="shared" si="0"/>
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="M4" s="17">
+        <v>0</v>
+      </c>
       <c r="N4" s="9">
         <v>42.617718000000004</v>
       </c>
@@ -699,16 +736,23 @@
       <c r="K5" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="L5" s="32">
+        <f t="shared" si="0"/>
+        <v>0.68835648148148143</v>
+      </c>
+      <c r="M5" s="17">
+        <v>1</v>
+      </c>
       <c r="N5" s="9">
         <v>42.617975999999999</v>
       </c>
       <c r="O5" s="9">
         <v>-92.312387999999999</v>
       </c>
-      <c r="P5" s="27" t="s">
+      <c r="P5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="28"/>
+      <c r="Q5" s="30"/>
       <c r="R5" s="10"/>
       <c r="S5" s="9">
         <v>42.617975999999999</v>
@@ -716,10 +760,10 @@
       <c r="T5" s="9">
         <v>-92.312387999999999</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="V5" s="28"/>
+      <c r="V5" s="30"/>
     </row>
     <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -755,17 +799,23 @@
       <c r="K6" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="28"/>
+      <c r="L6" s="32">
+        <f t="shared" si="0"/>
+        <v>0.69572916666666662</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
       <c r="N6" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O6" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="28"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="10"/>
       <c r="S6" s="9">
         <v>42.617718000000004</v>
@@ -812,17 +862,23 @@
       <c r="K7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="28"/>
+      <c r="L7" s="32">
+        <f t="shared" si="0"/>
+        <v>0.71043981481481477</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
       <c r="N7" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O7" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P7" s="27" t="s">
+      <c r="P7" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="28"/>
+      <c r="Q7" s="30"/>
       <c r="R7" s="10"/>
       <c r="S7" s="9">
         <v>42.590738000000002</v>
@@ -869,7 +925,13 @@
       <c r="K8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="28"/>
+      <c r="L8" s="32">
+        <f t="shared" si="0"/>
+        <v>0.71468750000000003</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
       <c r="N8" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -886,10 +948,10 @@
       <c r="T8" s="9">
         <v>-92.339399999999998</v>
       </c>
-      <c r="U8" s="27" t="s">
+      <c r="U8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="V8" s="28"/>
+      <c r="V8" s="30"/>
     </row>
     <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -925,16 +987,23 @@
       <c r="K9" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L9" s="32">
+        <f t="shared" si="0"/>
+        <v>0.72129629629629632</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
       <c r="N9" s="9">
         <v>42.592733000000003</v>
       </c>
       <c r="O9" s="9">
         <v>-92.336048000000005</v>
       </c>
-      <c r="P9" s="27" t="s">
+      <c r="P9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="28"/>
+      <c r="Q9" s="30"/>
       <c r="R9" s="10"/>
       <c r="S9" s="9">
         <v>42.625979999999998</v>
@@ -942,10 +1011,10 @@
       <c r="T9" s="9">
         <v>-92.338639999999998</v>
       </c>
-      <c r="U9" s="27" t="s">
+      <c r="U9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="V9" s="28"/>
+      <c r="V9" s="30"/>
     </row>
     <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -981,7 +1050,13 @@
       <c r="K10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="28"/>
+      <c r="L10" s="32">
+        <f t="shared" si="0"/>
+        <v>0.73306712962962961</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
       <c r="N10" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -998,10 +1073,10 @@
       <c r="T10" s="9">
         <v>-92.336048000000005</v>
       </c>
-      <c r="U10" s="27" t="s">
+      <c r="U10" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="V10" s="28"/>
+      <c r="V10" s="30"/>
     </row>
     <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -1037,6 +1112,13 @@
       <c r="K11" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L11" s="32">
+        <f t="shared" si="0"/>
+        <v>0.73803240740740739</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
       <c r="N11" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1053,10 +1135,10 @@
       <c r="T11" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="U11" s="27" t="s">
+      <c r="U11" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="V11" s="28"/>
+      <c r="V11" s="30"/>
     </row>
     <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -1092,16 +1174,23 @@
       <c r="K12" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.74159722222222224</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0</v>
+      </c>
       <c r="N12" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O12" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="28"/>
+      <c r="Q12" s="30"/>
     </row>
     <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -1137,17 +1226,23 @@
       <c r="K13" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="28"/>
+      <c r="L13" s="32">
+        <f t="shared" si="0"/>
+        <v>0.50873842592592589</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
       <c r="N13" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O13" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P13" s="27" t="s">
+      <c r="P13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q13" s="28"/>
+      <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -1183,7 +1278,13 @@
       <c r="K14" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="28"/>
+      <c r="L14" s="32">
+        <f t="shared" si="0"/>
+        <v>0.51208333333333333</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0</v>
+      </c>
       <c r="N14" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1228,6 +1329,13 @@
       <c r="K15" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L15" s="32">
+        <f t="shared" si="0"/>
+        <v>0.51758101851851857</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
       <c r="N15" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -1275,6 +1383,13 @@
       <c r="K16" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L16" s="32">
+        <f t="shared" si="0"/>
+        <v>0.5315509259259259</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
       <c r="N16" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -1322,6 +1437,13 @@
       <c r="K17" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L17" s="32">
+        <f t="shared" si="0"/>
+        <v>0.5366319444444444</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
       <c r="N17" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1367,16 +1489,23 @@
       <c r="K18" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L18" s="32">
+        <f t="shared" si="0"/>
+        <v>0.54052083333333334</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
       <c r="N18" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O18" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P18" s="27" t="s">
+      <c r="P18" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q18" s="28"/>
+      <c r="Q18" s="30"/>
       <c r="T18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1415,17 +1544,23 @@
       <c r="K19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="28"/>
+      <c r="L19" s="32">
+        <f t="shared" si="0"/>
+        <v>0.5590856481481481</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
       <c r="N19" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O19" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P19" s="27" t="s">
+      <c r="P19" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q19" s="28"/>
+      <c r="Q19" s="30"/>
       <c r="T19" s="5" t="s">
         <v>19</v>
       </c>
@@ -1464,7 +1599,13 @@
       <c r="K20" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L20" s="28"/>
+      <c r="L20" s="32">
+        <f t="shared" si="0"/>
+        <v>0.56206018518518519</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0</v>
+      </c>
       <c r="N20" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1509,6 +1650,13 @@
       <c r="K21" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L21" s="32">
+        <f t="shared" si="0"/>
+        <v>0.56765046296296295</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
       <c r="N21" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -1553,6 +1701,13 @@
       <c r="K22" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L22" s="32">
+        <f t="shared" si="0"/>
+        <v>0.58190972222222226</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0</v>
+      </c>
       <c r="N22" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -1597,6 +1752,13 @@
       <c r="K23" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L23" s="32">
+        <f t="shared" si="0"/>
+        <v>0.58674768518518516</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
       <c r="N23" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1641,16 +1803,23 @@
       <c r="K24" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L24" s="32">
+        <f t="shared" si="0"/>
+        <v>0.58987268518518521</v>
+      </c>
+      <c r="M24" s="9">
+        <v>0</v>
+      </c>
       <c r="N24" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O24" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P24" s="27" t="s">
+      <c r="P24" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q24" s="28"/>
+      <c r="Q24" s="30"/>
     </row>
     <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
@@ -1686,17 +1855,23 @@
       <c r="K25" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="28"/>
+      <c r="L25" s="32">
+        <f t="shared" si="0"/>
+        <v>0.62627314814814816</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
       <c r="N25" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O25" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P25" s="27" t="s">
+      <c r="P25" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q25" s="28"/>
+      <c r="Q25" s="30"/>
     </row>
     <row r="26" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -1732,7 +1907,13 @@
       <c r="K26" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L26" s="28"/>
+      <c r="L26" s="32">
+        <f t="shared" si="0"/>
+        <v>0.62959490740740742</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0</v>
+      </c>
       <c r="N26" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1777,6 +1958,13 @@
       <c r="K27" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L27" s="32">
+        <f t="shared" si="0"/>
+        <v>0.63517361111111115</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
       <c r="N27" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -1821,6 +2009,13 @@
       <c r="K28" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L28" s="32">
+        <f t="shared" si="0"/>
+        <v>0.65565972222222224</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0</v>
+      </c>
       <c r="N28" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -1865,6 +2060,13 @@
       <c r="K29" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L29" s="32">
+        <f t="shared" si="0"/>
+        <v>0.66137731481481477</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
       <c r="N29" s="9">
         <v>42.590738000000002</v>
       </c>
@@ -1909,16 +2111,23 @@
       <c r="K30" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="L30" s="32">
+        <f t="shared" si="0"/>
+        <v>0.66447916666666662</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0</v>
+      </c>
       <c r="N30" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O30" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P30" s="27" t="s">
+      <c r="P30" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q30" s="28"/>
+      <c r="Q30" s="30"/>
     </row>
     <row r="31" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
@@ -1954,17 +2163,23 @@
       <c r="K31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L31" s="28"/>
+      <c r="L31" s="32">
+        <f t="shared" si="0"/>
+        <v>0.51290509259259254</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
       <c r="N31" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O31" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P31" s="27" t="s">
+      <c r="P31" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q31" s="28"/>
+      <c r="Q31" s="30"/>
     </row>
     <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
@@ -2000,7 +2215,13 @@
       <c r="K32" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L32" s="28"/>
+      <c r="L32" s="32">
+        <f t="shared" si="0"/>
+        <v>0.51770833333333333</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0</v>
+      </c>
       <c r="N32" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -2045,6 +2266,13 @@
       <c r="K33" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L33" s="32">
+        <f t="shared" si="0"/>
+        <v>0.53156250000000005</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
       <c r="N33" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -2089,16 +2317,23 @@
       <c r="K34" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L34" s="32">
+        <f t="shared" si="0"/>
+        <v>0.53726851851851853</v>
+      </c>
+      <c r="M34" s="9">
+        <v>0</v>
+      </c>
       <c r="N34" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O34" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P34" s="27" t="s">
+      <c r="P34" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q34" s="28"/>
+      <c r="Q34" s="30"/>
     </row>
     <row r="35" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
@@ -2134,17 +2369,23 @@
       <c r="K35" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L35" s="28"/>
+      <c r="L35" s="32">
+        <f t="shared" si="0"/>
+        <v>0.59851851851851856</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
       <c r="N35" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O35" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P35" s="27" t="s">
+      <c r="P35" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q35" s="28"/>
+      <c r="Q35" s="30"/>
     </row>
     <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
@@ -2180,7 +2421,13 @@
       <c r="K36" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L36" s="28"/>
+      <c r="L36" s="32">
+        <f t="shared" si="0"/>
+        <v>0.60349537037037038</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0</v>
+      </c>
       <c r="N36" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -2225,6 +2472,13 @@
       <c r="K37" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L37" s="32">
+        <f t="shared" si="0"/>
+        <v>0.61285879629629625</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
+      </c>
       <c r="N37" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -2269,16 +2523,23 @@
       <c r="K38" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="L38" s="32">
+        <f t="shared" si="0"/>
+        <v>0.61744212962962963</v>
+      </c>
+      <c r="M38" s="9">
+        <v>0</v>
+      </c>
       <c r="N38" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O38" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P38" s="27" t="s">
+      <c r="P38" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q38" s="28"/>
+      <c r="Q38" s="30"/>
     </row>
     <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -2314,17 +2575,23 @@
       <c r="K39" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L39" s="28"/>
+      <c r="L39" s="32">
+        <f t="shared" si="0"/>
+        <v>0.46490740740740738</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
       <c r="N39" s="9">
         <v>42.588602000000002</v>
       </c>
       <c r="O39" s="9">
         <v>-92.332970000000003</v>
       </c>
-      <c r="P39" s="27" t="s">
+      <c r="P39" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="Q39" s="28"/>
+      <c r="Q39" s="30"/>
     </row>
     <row r="40" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
@@ -2360,7 +2627,13 @@
       <c r="K40" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L40" s="28"/>
+      <c r="L40" s="32">
+        <f t="shared" si="0"/>
+        <v>0.47064814814814815</v>
+      </c>
+      <c r="M40" s="9">
+        <v>0</v>
+      </c>
       <c r="N40" s="9">
         <v>42.592733000000003</v>
       </c>
@@ -2404,6 +2677,12 @@
       </c>
       <c r="K41" s="6" t="s">
         <v>30</v>
+      </c>
+      <c r="L41" s="32">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="M41" s="9">
+        <v>1</v>
       </c>
       <c r="N41" s="9">
         <v>42.592733000000003</v>
@@ -2429,8 +2708,8 @@
       <c r="K42" s="6"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="28"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="30"/>
     </row>
     <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
@@ -2447,8 +2726,8 @@
       <c r="L43" s="28"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="28"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="30"/>
     </row>
     <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
@@ -2478,7 +2757,8 @@
       <c r="H45" s="8"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
-      <c r="K45" s="6"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="28"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
       <c r="P45" s="6"/>
@@ -2494,11 +2774,12 @@
       <c r="H46" s="8"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
-      <c r="K46" s="6"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="28"/>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="28"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="30"/>
     </row>
     <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
@@ -2515,8 +2796,8 @@
       <c r="L47" s="28"/>
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
-      <c r="P47" s="27"/>
-      <c r="Q47" s="28"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="30"/>
     </row>
     <row r="48" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
@@ -2546,7 +2827,8 @@
       <c r="H49" s="8"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
-      <c r="K49" s="6"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="28"/>
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
       <c r="P49" s="6"/>
@@ -2562,11 +2844,12 @@
       <c r="H50" s="8"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
-      <c r="K50" s="6"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="28"/>
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
-      <c r="P50" s="27"/>
-      <c r="Q50" s="28"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="30"/>
     </row>
     <row r="51" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
@@ -2583,8 +2866,8 @@
       <c r="L51" s="28"/>
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
-      <c r="P51" s="27"/>
-      <c r="Q51" s="28"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="30"/>
     </row>
     <row r="52" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
@@ -2601,8 +2884,8 @@
       <c r="L52" s="28"/>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
-      <c r="P52" s="27"/>
-      <c r="Q52" s="28"/>
+      <c r="P52" s="29"/>
+      <c r="Q52" s="30"/>
     </row>
     <row r="53" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
@@ -2619,8 +2902,8 @@
       <c r="L53" s="28"/>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
-      <c r="P53" s="27"/>
-      <c r="Q53" s="28"/>
+      <c r="P53" s="29"/>
+      <c r="Q53" s="30"/>
     </row>
     <row r="54" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
@@ -2637,8 +2920,8 @@
       <c r="L54" s="28"/>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
-      <c r="P54" s="27"/>
-      <c r="Q54" s="28"/>
+      <c r="P54" s="29"/>
+      <c r="Q54" s="30"/>
     </row>
     <row r="55" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
@@ -2655,8 +2938,8 @@
       <c r="L55" s="28"/>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
-      <c r="P55" s="27"/>
-      <c r="Q55" s="28"/>
+      <c r="P55" s="29"/>
+      <c r="Q55" s="30"/>
     </row>
     <row r="56" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
@@ -2673,8 +2956,8 @@
       <c r="L56" s="28"/>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="28"/>
+      <c r="P56" s="29"/>
+      <c r="Q56" s="30"/>
     </row>
     <row r="57" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
@@ -2691,8 +2974,8 @@
       <c r="L57" s="28"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
-      <c r="P57" s="27"/>
-      <c r="Q57" s="28"/>
+      <c r="P57" s="29"/>
+      <c r="Q57" s="30"/>
     </row>
     <row r="58" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
@@ -2722,7 +3005,8 @@
       <c r="H59" s="8"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
-      <c r="K59" s="6"/>
+      <c r="K59" s="27"/>
+      <c r="L59" s="28"/>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
       <c r="P59" s="6"/>
@@ -2738,11 +3022,12 @@
       <c r="H60" s="8"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
-      <c r="K60" s="6"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="28"/>
       <c r="N60" s="9"/>
       <c r="O60" s="9"/>
-      <c r="P60" s="27"/>
-      <c r="Q60" s="28"/>
+      <c r="P60" s="29"/>
+      <c r="Q60" s="30"/>
     </row>
     <row r="61" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
@@ -2755,12 +3040,12 @@
       <c r="H61" s="8"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
-      <c r="K61" s="27"/>
-      <c r="L61" s="28"/>
+      <c r="K61" s="29"/>
+      <c r="L61" s="30"/>
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
-      <c r="P61" s="27"/>
-      <c r="Q61" s="28"/>
+      <c r="P61" s="29"/>
+      <c r="Q61" s="30"/>
     </row>
     <row r="62" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
@@ -2773,12 +3058,12 @@
       <c r="H62" s="8"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="28"/>
+      <c r="K62" s="29"/>
+      <c r="L62" s="30"/>
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
-      <c r="P62" s="27"/>
-      <c r="Q62" s="28"/>
+      <c r="P62" s="29"/>
+      <c r="Q62" s="30"/>
     </row>
     <row r="63" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
@@ -2791,12 +3076,12 @@
       <c r="H63" s="8"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="28"/>
+      <c r="K63" s="29"/>
+      <c r="L63" s="30"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
-      <c r="P63" s="27"/>
-      <c r="Q63" s="28"/>
+      <c r="P63" s="29"/>
+      <c r="Q63" s="30"/>
     </row>
     <row r="64" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
@@ -2809,12 +3094,12 @@
       <c r="H64" s="8"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="28"/>
+      <c r="K64" s="29"/>
+      <c r="L64" s="30"/>
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
-      <c r="P64" s="27"/>
-      <c r="Q64" s="28"/>
+      <c r="P64" s="29"/>
+      <c r="Q64" s="30"/>
     </row>
     <row r="65" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
@@ -2827,12 +3112,12 @@
       <c r="H65" s="8"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="28"/>
+      <c r="K65" s="29"/>
+      <c r="L65" s="30"/>
       <c r="N65" s="9"/>
       <c r="O65" s="9"/>
-      <c r="P65" s="27"/>
-      <c r="Q65" s="28"/>
+      <c r="P65" s="29"/>
+      <c r="Q65" s="30"/>
     </row>
     <row r="66" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
@@ -2845,12 +3130,12 @@
       <c r="H66" s="8"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="28"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="30"/>
       <c r="N66" s="9"/>
       <c r="O66" s="9"/>
-      <c r="P66" s="27"/>
-      <c r="Q66" s="28"/>
+      <c r="P66" s="29"/>
+      <c r="Q66" s="30"/>
     </row>
     <row r="67" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
@@ -2863,12 +3148,12 @@
       <c r="H67" s="8"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="28"/>
+      <c r="K67" s="29"/>
+      <c r="L67" s="30"/>
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
-      <c r="P67" s="27"/>
-      <c r="Q67" s="28"/>
+      <c r="P67" s="29"/>
+      <c r="Q67" s="30"/>
     </row>
     <row r="68" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
@@ -2881,12 +3166,12 @@
       <c r="H68" s="8"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
-      <c r="K68" s="27"/>
-      <c r="L68" s="28"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="30"/>
       <c r="N68" s="9"/>
       <c r="O68" s="9"/>
-      <c r="P68" s="27"/>
-      <c r="Q68" s="28"/>
+      <c r="P68" s="29"/>
+      <c r="Q68" s="30"/>
     </row>
     <row r="69" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
@@ -2899,12 +3184,12 @@
       <c r="H69" s="8"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="28"/>
+      <c r="K69" s="29"/>
+      <c r="L69" s="30"/>
       <c r="N69" s="9"/>
       <c r="O69" s="9"/>
-      <c r="P69" s="27"/>
-      <c r="Q69" s="28"/>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="30"/>
     </row>
     <row r="70" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
@@ -2917,12 +3202,12 @@
       <c r="H70" s="8"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
-      <c r="K70" s="27"/>
-      <c r="L70" s="28"/>
+      <c r="K70" s="29"/>
+      <c r="L70" s="30"/>
       <c r="N70" s="9"/>
       <c r="O70" s="9"/>
-      <c r="P70" s="27"/>
-      <c r="Q70" s="28"/>
+      <c r="P70" s="29"/>
+      <c r="Q70" s="30"/>
     </row>
     <row r="71" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
@@ -2935,12 +3220,12 @@
       <c r="H71" s="8"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
-      <c r="K71" s="27"/>
-      <c r="L71" s="28"/>
+      <c r="K71" s="29"/>
+      <c r="L71" s="30"/>
       <c r="N71" s="9"/>
       <c r="O71" s="9"/>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="28"/>
+      <c r="P71" s="29"/>
+      <c r="Q71" s="30"/>
     </row>
     <row r="72" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
@@ -2953,12 +3238,12 @@
       <c r="H72" s="8"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
-      <c r="K72" s="27"/>
-      <c r="L72" s="28"/>
+      <c r="K72" s="29"/>
+      <c r="L72" s="30"/>
       <c r="N72" s="9"/>
       <c r="O72" s="9"/>
-      <c r="P72" s="27"/>
-      <c r="Q72" s="28"/>
+      <c r="P72" s="29"/>
+      <c r="Q72" s="30"/>
     </row>
     <row r="73" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
@@ -2971,12 +3256,12 @@
       <c r="H73" s="8"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
-      <c r="K73" s="27"/>
-      <c r="L73" s="28"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="30"/>
       <c r="N73" s="9"/>
       <c r="O73" s="9"/>
-      <c r="P73" s="27"/>
-      <c r="Q73" s="28"/>
+      <c r="P73" s="29"/>
+      <c r="Q73" s="30"/>
     </row>
     <row r="74" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
@@ -2989,8 +3274,8 @@
       <c r="H74" s="8"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
-      <c r="K74" s="27"/>
-      <c r="L74" s="28"/>
+      <c r="K74" s="29"/>
+      <c r="L74" s="30"/>
       <c r="N74" s="9"/>
       <c r="O74" s="9"/>
       <c r="P74" s="6"/>
@@ -3025,8 +3310,8 @@
       <c r="K76" s="6"/>
       <c r="N76" s="9"/>
       <c r="O76" s="9"/>
-      <c r="P76" s="27"/>
-      <c r="Q76" s="28"/>
+      <c r="P76" s="29"/>
+      <c r="Q76" s="30"/>
     </row>
     <row r="77" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
@@ -3039,12 +3324,12 @@
       <c r="H77" s="8"/>
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
-      <c r="K77" s="27"/>
-      <c r="L77" s="28"/>
+      <c r="K77" s="29"/>
+      <c r="L77" s="30"/>
       <c r="N77" s="9"/>
       <c r="O77" s="9"/>
-      <c r="P77" s="27"/>
-      <c r="Q77" s="28"/>
+      <c r="P77" s="29"/>
+      <c r="Q77" s="30"/>
     </row>
     <row r="78" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
@@ -3057,8 +3342,8 @@
       <c r="H78" s="8"/>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
-      <c r="K78" s="27"/>
-      <c r="L78" s="28"/>
+      <c r="K78" s="29"/>
+      <c r="L78" s="30"/>
       <c r="N78" s="9"/>
       <c r="O78" s="9"/>
       <c r="P78" s="6"/>
@@ -3125,8 +3410,8 @@
       <c r="K82" s="6"/>
       <c r="N82" s="9"/>
       <c r="O82" s="9"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="28"/>
+      <c r="P82" s="29"/>
+      <c r="Q82" s="30"/>
     </row>
     <row r="83" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
@@ -3139,12 +3424,12 @@
       <c r="H83" s="8"/>
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="28"/>
+      <c r="K83" s="29"/>
+      <c r="L83" s="30"/>
       <c r="N83" s="9"/>
       <c r="O83" s="9"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="28"/>
+      <c r="P83" s="29"/>
+      <c r="Q83" s="30"/>
     </row>
     <row r="84" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
@@ -3157,12 +3442,12 @@
       <c r="H84" s="8"/>
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
-      <c r="K84" s="27"/>
-      <c r="L84" s="28"/>
+      <c r="K84" s="29"/>
+      <c r="L84" s="30"/>
       <c r="N84" s="9"/>
       <c r="O84" s="9"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="28"/>
+      <c r="P84" s="29"/>
+      <c r="Q84" s="30"/>
     </row>
     <row r="85" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="5"/>
@@ -3175,12 +3460,12 @@
       <c r="H85" s="8"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
-      <c r="K85" s="27"/>
-      <c r="L85" s="28"/>
+      <c r="K85" s="29"/>
+      <c r="L85" s="30"/>
       <c r="N85" s="9"/>
       <c r="O85" s="9"/>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="28"/>
+      <c r="P85" s="29"/>
+      <c r="Q85" s="30"/>
     </row>
     <row r="86" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
@@ -3193,12 +3478,12 @@
       <c r="H86" s="8"/>
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
-      <c r="K86" s="27"/>
-      <c r="L86" s="28"/>
+      <c r="K86" s="29"/>
+      <c r="L86" s="30"/>
       <c r="N86" s="9"/>
       <c r="O86" s="9"/>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="28"/>
+      <c r="P86" s="29"/>
+      <c r="Q86" s="30"/>
     </row>
     <row r="87" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
@@ -3211,12 +3496,12 @@
       <c r="H87" s="8"/>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
-      <c r="K87" s="27"/>
-      <c r="L87" s="28"/>
+      <c r="K87" s="29"/>
+      <c r="L87" s="30"/>
       <c r="N87" s="9"/>
       <c r="O87" s="9"/>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="28"/>
+      <c r="P87" s="29"/>
+      <c r="Q87" s="30"/>
     </row>
     <row r="88" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
@@ -3229,8 +3514,8 @@
       <c r="H88" s="8"/>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
-      <c r="K88" s="27"/>
-      <c r="L88" s="28"/>
+      <c r="K88" s="29"/>
+      <c r="L88" s="30"/>
       <c r="N88" s="9"/>
       <c r="O88" s="9"/>
       <c r="P88" s="6"/>
@@ -3265,8 +3550,8 @@
       <c r="K90" s="6"/>
       <c r="N90" s="9"/>
       <c r="O90" s="9"/>
-      <c r="P90" s="27"/>
-      <c r="Q90" s="28"/>
+      <c r="P90" s="29"/>
+      <c r="Q90" s="30"/>
     </row>
     <row r="91" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
@@ -3279,12 +3564,12 @@
       <c r="H91" s="8"/>
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="28"/>
+      <c r="K91" s="29"/>
+      <c r="L91" s="30"/>
       <c r="N91" s="9"/>
       <c r="O91" s="9"/>
-      <c r="P91" s="27"/>
-      <c r="Q91" s="28"/>
+      <c r="P91" s="29"/>
+      <c r="Q91" s="30"/>
     </row>
     <row r="92" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
@@ -3297,12 +3582,12 @@
       <c r="H92" s="8"/>
       <c r="I92" s="9"/>
       <c r="J92" s="9"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="28"/>
+      <c r="K92" s="29"/>
+      <c r="L92" s="30"/>
       <c r="N92" s="9"/>
       <c r="O92" s="9"/>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="28"/>
+      <c r="P92" s="29"/>
+      <c r="Q92" s="30"/>
     </row>
     <row r="93" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
@@ -3315,12 +3600,12 @@
       <c r="H93" s="8"/>
       <c r="I93" s="9"/>
       <c r="J93" s="9"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="28"/>
+      <c r="K93" s="29"/>
+      <c r="L93" s="30"/>
       <c r="N93" s="9"/>
       <c r="O93" s="9"/>
-      <c r="P93" s="27"/>
-      <c r="Q93" s="28"/>
+      <c r="P93" s="29"/>
+      <c r="Q93" s="30"/>
     </row>
     <row r="94" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
@@ -3333,12 +3618,12 @@
       <c r="H94" s="8"/>
       <c r="I94" s="9"/>
       <c r="J94" s="9"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="28"/>
+      <c r="K94" s="29"/>
+      <c r="L94" s="30"/>
       <c r="N94" s="9"/>
       <c r="O94" s="9"/>
-      <c r="P94" s="27"/>
-      <c r="Q94" s="28"/>
+      <c r="P94" s="29"/>
+      <c r="Q94" s="30"/>
     </row>
     <row r="95" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
@@ -3351,12 +3636,12 @@
       <c r="H95" s="8"/>
       <c r="I95" s="9"/>
       <c r="J95" s="9"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="28"/>
+      <c r="K95" s="29"/>
+      <c r="L95" s="30"/>
       <c r="N95" s="9"/>
       <c r="O95" s="9"/>
-      <c r="P95" s="27"/>
-      <c r="Q95" s="28"/>
+      <c r="P95" s="29"/>
+      <c r="Q95" s="30"/>
     </row>
     <row r="96" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
@@ -3369,8 +3654,8 @@
       <c r="H96" s="8"/>
       <c r="I96" s="9"/>
       <c r="J96" s="9"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="28"/>
+      <c r="K96" s="29"/>
+      <c r="L96" s="30"/>
       <c r="N96" s="9"/>
       <c r="O96" s="9"/>
       <c r="P96" s="6"/>
@@ -3405,8 +3690,8 @@
       <c r="K98" s="6"/>
       <c r="N98" s="9"/>
       <c r="O98" s="9"/>
-      <c r="P98" s="27"/>
-      <c r="Q98" s="28"/>
+      <c r="P98" s="29"/>
+      <c r="Q98" s="30"/>
     </row>
     <row r="99" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
@@ -3419,12 +3704,12 @@
       <c r="H99" s="8"/>
       <c r="I99" s="9"/>
       <c r="J99" s="9"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="28"/>
+      <c r="K99" s="29"/>
+      <c r="L99" s="30"/>
       <c r="N99" s="9"/>
       <c r="O99" s="9"/>
-      <c r="P99" s="27"/>
-      <c r="Q99" s="28"/>
+      <c r="P99" s="29"/>
+      <c r="Q99" s="30"/>
     </row>
     <row r="100" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
@@ -3437,12 +3722,12 @@
       <c r="H100" s="8"/>
       <c r="I100" s="9"/>
       <c r="J100" s="9"/>
-      <c r="K100" s="27"/>
-      <c r="L100" s="28"/>
+      <c r="K100" s="29"/>
+      <c r="L100" s="30"/>
       <c r="N100" s="9"/>
       <c r="O100" s="9"/>
-      <c r="P100" s="27"/>
-      <c r="Q100" s="28"/>
+      <c r="P100" s="29"/>
+      <c r="Q100" s="30"/>
     </row>
     <row r="101" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
@@ -3455,12 +3740,12 @@
       <c r="H101" s="8"/>
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="28"/>
+      <c r="K101" s="29"/>
+      <c r="L101" s="30"/>
       <c r="N101" s="9"/>
       <c r="O101" s="9"/>
-      <c r="P101" s="27"/>
-      <c r="Q101" s="28"/>
+      <c r="P101" s="29"/>
+      <c r="Q101" s="30"/>
     </row>
     <row r="102" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
@@ -3473,12 +3758,12 @@
       <c r="H102" s="8"/>
       <c r="I102" s="9"/>
       <c r="J102" s="9"/>
-      <c r="K102" s="27"/>
-      <c r="L102" s="28"/>
+      <c r="K102" s="29"/>
+      <c r="L102" s="30"/>
       <c r="N102" s="9"/>
       <c r="O102" s="9"/>
-      <c r="P102" s="27"/>
-      <c r="Q102" s="28"/>
+      <c r="P102" s="29"/>
+      <c r="Q102" s="30"/>
     </row>
     <row r="103" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
@@ -3491,12 +3776,12 @@
       <c r="H103" s="8"/>
       <c r="I103" s="9"/>
       <c r="J103" s="9"/>
-      <c r="K103" s="27"/>
-      <c r="L103" s="28"/>
+      <c r="K103" s="29"/>
+      <c r="L103" s="30"/>
       <c r="N103" s="9"/>
       <c r="O103" s="9"/>
-      <c r="P103" s="27"/>
-      <c r="Q103" s="28"/>
+      <c r="P103" s="29"/>
+      <c r="Q103" s="30"/>
     </row>
     <row r="104" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
@@ -3509,12 +3794,12 @@
       <c r="H104" s="8"/>
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
-      <c r="K104" s="27"/>
-      <c r="L104" s="28"/>
+      <c r="K104" s="29"/>
+      <c r="L104" s="30"/>
       <c r="N104" s="9"/>
       <c r="O104" s="9"/>
-      <c r="P104" s="27"/>
-      <c r="Q104" s="28"/>
+      <c r="P104" s="29"/>
+      <c r="Q104" s="30"/>
     </row>
     <row r="105" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="5"/>
@@ -3527,12 +3812,12 @@
       <c r="H105" s="8"/>
       <c r="I105" s="9"/>
       <c r="J105" s="9"/>
-      <c r="K105" s="27"/>
-      <c r="L105" s="28"/>
+      <c r="K105" s="29"/>
+      <c r="L105" s="30"/>
       <c r="N105" s="9"/>
       <c r="O105" s="9"/>
-      <c r="P105" s="27"/>
-      <c r="Q105" s="28"/>
+      <c r="P105" s="29"/>
+      <c r="Q105" s="30"/>
     </row>
     <row r="106" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
@@ -3545,12 +3830,12 @@
       <c r="H106" s="8"/>
       <c r="I106" s="9"/>
       <c r="J106" s="9"/>
-      <c r="K106" s="27"/>
-      <c r="L106" s="28"/>
+      <c r="K106" s="29"/>
+      <c r="L106" s="30"/>
       <c r="N106" s="9"/>
       <c r="O106" s="9"/>
-      <c r="P106" s="27"/>
-      <c r="Q106" s="28"/>
+      <c r="P106" s="29"/>
+      <c r="Q106" s="30"/>
     </row>
     <row r="107" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
@@ -3563,12 +3848,12 @@
       <c r="H107" s="8"/>
       <c r="I107" s="9"/>
       <c r="J107" s="9"/>
-      <c r="K107" s="27"/>
-      <c r="L107" s="28"/>
+      <c r="K107" s="29"/>
+      <c r="L107" s="30"/>
       <c r="N107" s="9"/>
       <c r="O107" s="9"/>
-      <c r="P107" s="27"/>
-      <c r="Q107" s="28"/>
+      <c r="P107" s="29"/>
+      <c r="Q107" s="30"/>
     </row>
     <row r="108" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="5"/>
@@ -3581,12 +3866,12 @@
       <c r="H108" s="8"/>
       <c r="I108" s="9"/>
       <c r="J108" s="9"/>
-      <c r="K108" s="27"/>
-      <c r="L108" s="28"/>
+      <c r="K108" s="29"/>
+      <c r="L108" s="30"/>
       <c r="N108" s="9"/>
       <c r="O108" s="9"/>
-      <c r="P108" s="27"/>
-      <c r="Q108" s="28"/>
+      <c r="P108" s="29"/>
+      <c r="Q108" s="30"/>
     </row>
     <row r="109" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
@@ -3599,12 +3884,12 @@
       <c r="H109" s="8"/>
       <c r="I109" s="9"/>
       <c r="J109" s="9"/>
-      <c r="K109" s="27"/>
-      <c r="L109" s="28"/>
+      <c r="K109" s="29"/>
+      <c r="L109" s="30"/>
       <c r="N109" s="9"/>
       <c r="O109" s="9"/>
-      <c r="P109" s="27"/>
-      <c r="Q109" s="28"/>
+      <c r="P109" s="29"/>
+      <c r="Q109" s="30"/>
     </row>
     <row r="110" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
@@ -3617,12 +3902,12 @@
       <c r="H110" s="8"/>
       <c r="I110" s="9"/>
       <c r="J110" s="9"/>
-      <c r="K110" s="27"/>
-      <c r="L110" s="28"/>
+      <c r="K110" s="29"/>
+      <c r="L110" s="30"/>
       <c r="N110" s="9"/>
       <c r="O110" s="9"/>
-      <c r="P110" s="27"/>
-      <c r="Q110" s="28"/>
+      <c r="P110" s="29"/>
+      <c r="Q110" s="30"/>
     </row>
     <row r="111" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="5"/>
@@ -3635,12 +3920,12 @@
       <c r="H111" s="8"/>
       <c r="I111" s="9"/>
       <c r="J111" s="9"/>
-      <c r="K111" s="27"/>
-      <c r="L111" s="28"/>
+      <c r="K111" s="29"/>
+      <c r="L111" s="30"/>
       <c r="N111" s="9"/>
       <c r="O111" s="9"/>
-      <c r="P111" s="27"/>
-      <c r="Q111" s="28"/>
+      <c r="P111" s="29"/>
+      <c r="Q111" s="30"/>
     </row>
     <row r="112" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
@@ -3653,8 +3938,8 @@
       <c r="H112" s="8"/>
       <c r="I112" s="9"/>
       <c r="J112" s="9"/>
-      <c r="K112" s="27"/>
-      <c r="L112" s="28"/>
+      <c r="K112" s="29"/>
+      <c r="L112" s="30"/>
       <c r="N112" s="9"/>
       <c r="O112" s="9"/>
       <c r="P112" s="6"/>
@@ -3689,8 +3974,8 @@
       <c r="K114" s="6"/>
       <c r="N114" s="9"/>
       <c r="O114" s="9"/>
-      <c r="P114" s="27"/>
-      <c r="Q114" s="28"/>
+      <c r="P114" s="29"/>
+      <c r="Q114" s="30"/>
     </row>
     <row r="115" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="5"/>
@@ -3703,12 +3988,12 @@
       <c r="H115" s="8"/>
       <c r="I115" s="9"/>
       <c r="J115" s="9"/>
-      <c r="K115" s="27"/>
-      <c r="L115" s="28"/>
+      <c r="K115" s="29"/>
+      <c r="L115" s="30"/>
       <c r="N115" s="9"/>
       <c r="O115" s="9"/>
-      <c r="P115" s="27"/>
-      <c r="Q115" s="28"/>
+      <c r="P115" s="29"/>
+      <c r="Q115" s="30"/>
     </row>
     <row r="116" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="5"/>
@@ -3721,12 +4006,12 @@
       <c r="H116" s="8"/>
       <c r="I116" s="9"/>
       <c r="J116" s="9"/>
-      <c r="K116" s="27"/>
-      <c r="L116" s="28"/>
+      <c r="K116" s="29"/>
+      <c r="L116" s="30"/>
       <c r="N116" s="9"/>
       <c r="O116" s="9"/>
-      <c r="P116" s="27"/>
-      <c r="Q116" s="28"/>
+      <c r="P116" s="29"/>
+      <c r="Q116" s="30"/>
     </row>
     <row r="117" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="5"/>
@@ -3739,12 +4024,12 @@
       <c r="H117" s="8"/>
       <c r="I117" s="9"/>
       <c r="J117" s="9"/>
-      <c r="K117" s="27"/>
-      <c r="L117" s="28"/>
+      <c r="K117" s="29"/>
+      <c r="L117" s="30"/>
       <c r="N117" s="9"/>
       <c r="O117" s="9"/>
-      <c r="P117" s="27"/>
-      <c r="Q117" s="28"/>
+      <c r="P117" s="29"/>
+      <c r="Q117" s="30"/>
     </row>
     <row r="118" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="5"/>
@@ -3757,12 +4042,12 @@
       <c r="H118" s="8"/>
       <c r="I118" s="9"/>
       <c r="J118" s="9"/>
-      <c r="K118" s="27"/>
-      <c r="L118" s="28"/>
+      <c r="K118" s="29"/>
+      <c r="L118" s="30"/>
       <c r="N118" s="9"/>
       <c r="O118" s="9"/>
-      <c r="P118" s="27"/>
-      <c r="Q118" s="28"/>
+      <c r="P118" s="29"/>
+      <c r="Q118" s="30"/>
     </row>
     <row r="119" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A119" s="5"/>
@@ -3775,12 +4060,12 @@
       <c r="H119" s="8"/>
       <c r="I119" s="9"/>
       <c r="J119" s="9"/>
-      <c r="K119" s="27"/>
-      <c r="L119" s="28"/>
+      <c r="K119" s="29"/>
+      <c r="L119" s="30"/>
       <c r="N119" s="9"/>
       <c r="O119" s="9"/>
-      <c r="P119" s="27"/>
-      <c r="Q119" s="28"/>
+      <c r="P119" s="29"/>
+      <c r="Q119" s="30"/>
     </row>
     <row r="120" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="5"/>
@@ -3793,12 +4078,12 @@
       <c r="H120" s="8"/>
       <c r="I120" s="9"/>
       <c r="J120" s="9"/>
-      <c r="K120" s="27"/>
-      <c r="L120" s="28"/>
+      <c r="K120" s="29"/>
+      <c r="L120" s="30"/>
       <c r="N120" s="9"/>
       <c r="O120" s="9"/>
-      <c r="P120" s="27"/>
-      <c r="Q120" s="28"/>
+      <c r="P120" s="29"/>
+      <c r="Q120" s="30"/>
     </row>
     <row r="121" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" s="5"/>
@@ -3811,12 +4096,12 @@
       <c r="H121" s="8"/>
       <c r="I121" s="9"/>
       <c r="J121" s="9"/>
-      <c r="K121" s="27"/>
-      <c r="L121" s="28"/>
+      <c r="K121" s="29"/>
+      <c r="L121" s="30"/>
       <c r="N121" s="9"/>
       <c r="O121" s="9"/>
-      <c r="P121" s="27"/>
-      <c r="Q121" s="28"/>
+      <c r="P121" s="29"/>
+      <c r="Q121" s="30"/>
     </row>
     <row r="122" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A122" s="5"/>
@@ -3829,8 +4114,8 @@
       <c r="H122" s="8"/>
       <c r="I122" s="9"/>
       <c r="J122" s="9"/>
-      <c r="K122" s="27"/>
-      <c r="L122" s="28"/>
+      <c r="K122" s="29"/>
+      <c r="L122" s="30"/>
       <c r="N122" s="9"/>
       <c r="O122" s="9"/>
       <c r="P122" s="6"/>
@@ -3865,8 +4150,8 @@
       <c r="K124" s="6"/>
       <c r="N124" s="9"/>
       <c r="O124" s="9"/>
-      <c r="P124" s="27"/>
-      <c r="Q124" s="28"/>
+      <c r="P124" s="29"/>
+      <c r="Q124" s="30"/>
     </row>
     <row r="125" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="5"/>
@@ -3879,12 +4164,12 @@
       <c r="H125" s="8"/>
       <c r="I125" s="9"/>
       <c r="J125" s="9"/>
-      <c r="K125" s="27"/>
-      <c r="L125" s="28"/>
+      <c r="K125" s="29"/>
+      <c r="L125" s="30"/>
       <c r="N125" s="9"/>
       <c r="O125" s="9"/>
-      <c r="P125" s="27"/>
-      <c r="Q125" s="28"/>
+      <c r="P125" s="29"/>
+      <c r="Q125" s="30"/>
     </row>
     <row r="126" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="5"/>
@@ -3897,12 +4182,12 @@
       <c r="H126" s="8"/>
       <c r="I126" s="9"/>
       <c r="J126" s="9"/>
-      <c r="K126" s="27"/>
-      <c r="L126" s="28"/>
+      <c r="K126" s="29"/>
+      <c r="L126" s="30"/>
       <c r="N126" s="9"/>
       <c r="O126" s="9"/>
-      <c r="P126" s="27"/>
-      <c r="Q126" s="28"/>
+      <c r="P126" s="29"/>
+      <c r="Q126" s="30"/>
     </row>
     <row r="127" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="5"/>
@@ -3915,12 +4200,12 @@
       <c r="H127" s="8"/>
       <c r="I127" s="9"/>
       <c r="J127" s="9"/>
-      <c r="K127" s="27"/>
-      <c r="L127" s="28"/>
+      <c r="K127" s="29"/>
+      <c r="L127" s="30"/>
       <c r="N127" s="9"/>
       <c r="O127" s="9"/>
-      <c r="P127" s="27"/>
-      <c r="Q127" s="28"/>
+      <c r="P127" s="29"/>
+      <c r="Q127" s="30"/>
     </row>
     <row r="128" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A128" s="5"/>
@@ -3933,12 +4218,12 @@
       <c r="H128" s="8"/>
       <c r="I128" s="9"/>
       <c r="J128" s="9"/>
-      <c r="K128" s="27"/>
-      <c r="L128" s="28"/>
+      <c r="K128" s="29"/>
+      <c r="L128" s="30"/>
       <c r="N128" s="9"/>
       <c r="O128" s="9"/>
-      <c r="P128" s="27"/>
-      <c r="Q128" s="28"/>
+      <c r="P128" s="29"/>
+      <c r="Q128" s="30"/>
     </row>
     <row r="129" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A129" s="5"/>
@@ -3951,12 +4236,12 @@
       <c r="H129" s="8"/>
       <c r="I129" s="9"/>
       <c r="J129" s="9"/>
-      <c r="K129" s="27"/>
-      <c r="L129" s="28"/>
+      <c r="K129" s="29"/>
+      <c r="L129" s="30"/>
       <c r="N129" s="9"/>
       <c r="O129" s="9"/>
-      <c r="P129" s="27"/>
-      <c r="Q129" s="28"/>
+      <c r="P129" s="29"/>
+      <c r="Q129" s="30"/>
     </row>
     <row r="130" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A130" s="5"/>
@@ -3969,12 +4254,12 @@
       <c r="H130" s="8"/>
       <c r="I130" s="9"/>
       <c r="J130" s="9"/>
-      <c r="K130" s="27"/>
-      <c r="L130" s="28"/>
+      <c r="K130" s="29"/>
+      <c r="L130" s="30"/>
       <c r="N130" s="9"/>
       <c r="O130" s="9"/>
-      <c r="P130" s="27"/>
-      <c r="Q130" s="28"/>
+      <c r="P130" s="29"/>
+      <c r="Q130" s="30"/>
     </row>
     <row r="131" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
@@ -3987,12 +4272,12 @@
       <c r="H131" s="8"/>
       <c r="I131" s="9"/>
       <c r="J131" s="9"/>
-      <c r="K131" s="27"/>
-      <c r="L131" s="28"/>
+      <c r="K131" s="29"/>
+      <c r="L131" s="30"/>
       <c r="N131" s="9"/>
       <c r="O131" s="9"/>
-      <c r="P131" s="27"/>
-      <c r="Q131" s="28"/>
+      <c r="P131" s="29"/>
+      <c r="Q131" s="30"/>
     </row>
     <row r="132" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A132" s="5"/>
@@ -4005,12 +4290,12 @@
       <c r="H132" s="8"/>
       <c r="I132" s="9"/>
       <c r="J132" s="9"/>
-      <c r="K132" s="27"/>
-      <c r="L132" s="28"/>
+      <c r="K132" s="29"/>
+      <c r="L132" s="30"/>
       <c r="N132" s="9"/>
       <c r="O132" s="9"/>
-      <c r="P132" s="27"/>
-      <c r="Q132" s="28"/>
+      <c r="P132" s="29"/>
+      <c r="Q132" s="30"/>
     </row>
     <row r="133" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A133" s="5"/>
@@ -4023,12 +4308,12 @@
       <c r="H133" s="8"/>
       <c r="I133" s="9"/>
       <c r="J133" s="9"/>
-      <c r="K133" s="27"/>
-      <c r="L133" s="28"/>
+      <c r="K133" s="29"/>
+      <c r="L133" s="30"/>
       <c r="N133" s="9"/>
       <c r="O133" s="9"/>
-      <c r="P133" s="27"/>
-      <c r="Q133" s="28"/>
+      <c r="P133" s="29"/>
+      <c r="Q133" s="30"/>
     </row>
     <row r="134" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
@@ -4041,12 +4326,12 @@
       <c r="H134" s="8"/>
       <c r="I134" s="9"/>
       <c r="J134" s="9"/>
-      <c r="K134" s="27"/>
-      <c r="L134" s="28"/>
+      <c r="K134" s="29"/>
+      <c r="L134" s="30"/>
       <c r="N134" s="9"/>
       <c r="O134" s="9"/>
-      <c r="P134" s="27"/>
-      <c r="Q134" s="28"/>
+      <c r="P134" s="29"/>
+      <c r="Q134" s="30"/>
     </row>
     <row r="135" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A135" s="5"/>
@@ -4059,12 +4344,12 @@
       <c r="H135" s="8"/>
       <c r="I135" s="9"/>
       <c r="J135" s="9"/>
-      <c r="K135" s="27"/>
-      <c r="L135" s="28"/>
+      <c r="K135" s="29"/>
+      <c r="L135" s="30"/>
       <c r="N135" s="9"/>
       <c r="O135" s="9"/>
-      <c r="P135" s="27"/>
-      <c r="Q135" s="28"/>
+      <c r="P135" s="29"/>
+      <c r="Q135" s="30"/>
     </row>
     <row r="136" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="5"/>
@@ -4077,12 +4362,12 @@
       <c r="H136" s="8"/>
       <c r="I136" s="9"/>
       <c r="J136" s="9"/>
-      <c r="K136" s="27"/>
-      <c r="L136" s="28"/>
+      <c r="K136" s="29"/>
+      <c r="L136" s="30"/>
       <c r="N136" s="9"/>
       <c r="O136" s="9"/>
-      <c r="P136" s="27"/>
-      <c r="Q136" s="28"/>
+      <c r="P136" s="29"/>
+      <c r="Q136" s="30"/>
     </row>
     <row r="137" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="5"/>
@@ -4095,12 +4380,12 @@
       <c r="H137" s="8"/>
       <c r="I137" s="9"/>
       <c r="J137" s="9"/>
-      <c r="K137" s="27"/>
-      <c r="L137" s="28"/>
+      <c r="K137" s="29"/>
+      <c r="L137" s="30"/>
       <c r="N137" s="9"/>
       <c r="O137" s="9"/>
-      <c r="P137" s="27"/>
-      <c r="Q137" s="28"/>
+      <c r="P137" s="29"/>
+      <c r="Q137" s="30"/>
     </row>
     <row r="138" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A138" s="5"/>
@@ -4113,8 +4398,8 @@
       <c r="H138" s="8"/>
       <c r="I138" s="9"/>
       <c r="J138" s="9"/>
-      <c r="K138" s="27"/>
-      <c r="L138" s="28"/>
+      <c r="K138" s="29"/>
+      <c r="L138" s="30"/>
       <c r="N138" s="9"/>
       <c r="O138" s="9"/>
       <c r="P138" s="6"/>
@@ -4149,8 +4434,8 @@
       <c r="K140" s="6"/>
       <c r="N140" s="9"/>
       <c r="O140" s="9"/>
-      <c r="P140" s="27"/>
-      <c r="Q140" s="28"/>
+      <c r="P140" s="29"/>
+      <c r="Q140" s="30"/>
     </row>
     <row r="141" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A141" s="5"/>
@@ -4163,12 +4448,12 @@
       <c r="H141" s="8"/>
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
-      <c r="K141" s="27"/>
-      <c r="L141" s="28"/>
+      <c r="K141" s="29"/>
+      <c r="L141" s="30"/>
       <c r="N141" s="9"/>
       <c r="O141" s="9"/>
-      <c r="P141" s="27"/>
-      <c r="Q141" s="28"/>
+      <c r="P141" s="29"/>
+      <c r="Q141" s="30"/>
     </row>
     <row r="142" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A142" s="5"/>
@@ -4181,8 +4466,8 @@
       <c r="H142" s="8"/>
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
-      <c r="K142" s="27"/>
-      <c r="L142" s="28"/>
+      <c r="K142" s="29"/>
+      <c r="L142" s="30"/>
       <c r="N142" s="9"/>
       <c r="O142" s="9"/>
       <c r="P142" s="6"/>
@@ -4217,8 +4502,8 @@
       <c r="K144" s="6"/>
       <c r="N144" s="9"/>
       <c r="O144" s="9"/>
-      <c r="P144" s="27"/>
-      <c r="Q144" s="28"/>
+      <c r="P144" s="29"/>
+      <c r="Q144" s="30"/>
     </row>
     <row r="145" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A145" s="5"/>
@@ -4231,12 +4516,12 @@
       <c r="H145" s="8"/>
       <c r="I145" s="9"/>
       <c r="J145" s="9"/>
-      <c r="K145" s="27"/>
-      <c r="L145" s="28"/>
+      <c r="K145" s="29"/>
+      <c r="L145" s="30"/>
       <c r="N145" s="9"/>
       <c r="O145" s="9"/>
-      <c r="P145" s="27"/>
-      <c r="Q145" s="28"/>
+      <c r="P145" s="29"/>
+      <c r="Q145" s="30"/>
     </row>
     <row r="146" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A146" s="5"/>
@@ -4249,8 +4534,8 @@
       <c r="H146" s="8"/>
       <c r="I146" s="9"/>
       <c r="J146" s="9"/>
-      <c r="K146" s="27"/>
-      <c r="L146" s="28"/>
+      <c r="K146" s="29"/>
+      <c r="L146" s="30"/>
       <c r="N146" s="9"/>
       <c r="O146" s="9"/>
       <c r="P146" s="6"/>
@@ -4285,8 +4570,8 @@
       <c r="K148" s="6"/>
       <c r="N148" s="9"/>
       <c r="O148" s="9"/>
-      <c r="P148" s="27"/>
-      <c r="Q148" s="28"/>
+      <c r="P148" s="29"/>
+      <c r="Q148" s="30"/>
     </row>
     <row r="149" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A149" s="5"/>
@@ -4299,12 +4584,12 @@
       <c r="H149" s="8"/>
       <c r="I149" s="9"/>
       <c r="J149" s="9"/>
-      <c r="K149" s="27"/>
-      <c r="L149" s="28"/>
+      <c r="K149" s="29"/>
+      <c r="L149" s="30"/>
       <c r="N149" s="9"/>
       <c r="O149" s="9"/>
-      <c r="P149" s="27"/>
-      <c r="Q149" s="28"/>
+      <c r="P149" s="29"/>
+      <c r="Q149" s="30"/>
     </row>
     <row r="150" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A150" s="5"/>
@@ -4317,8 +4602,8 @@
       <c r="H150" s="8"/>
       <c r="I150" s="9"/>
       <c r="J150" s="9"/>
-      <c r="K150" s="27"/>
-      <c r="L150" s="28"/>
+      <c r="K150" s="29"/>
+      <c r="L150" s="30"/>
       <c r="N150" s="9"/>
       <c r="O150" s="9"/>
       <c r="P150" s="6"/>
@@ -4353,8 +4638,8 @@
       <c r="K152" s="6"/>
       <c r="N152" s="9"/>
       <c r="O152" s="9"/>
-      <c r="P152" s="27"/>
-      <c r="Q152" s="28"/>
+      <c r="P152" s="29"/>
+      <c r="Q152" s="30"/>
     </row>
     <row r="153" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A153" s="5"/>
@@ -4367,12 +4652,12 @@
       <c r="H153" s="8"/>
       <c r="I153" s="9"/>
       <c r="J153" s="9"/>
-      <c r="K153" s="27"/>
-      <c r="L153" s="28"/>
+      <c r="K153" s="29"/>
+      <c r="L153" s="30"/>
       <c r="N153" s="9"/>
       <c r="O153" s="9"/>
-      <c r="P153" s="27"/>
-      <c r="Q153" s="28"/>
+      <c r="P153" s="29"/>
+      <c r="Q153" s="30"/>
     </row>
     <row r="154" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A154" s="5"/>
@@ -4385,8 +4670,8 @@
       <c r="H154" s="8"/>
       <c r="I154" s="9"/>
       <c r="J154" s="9"/>
-      <c r="K154" s="27"/>
-      <c r="L154" s="28"/>
+      <c r="K154" s="29"/>
+      <c r="L154" s="30"/>
       <c r="N154" s="9"/>
       <c r="O154" s="9"/>
       <c r="P154" s="6"/>
@@ -4421,8 +4706,8 @@
       <c r="K156" s="6"/>
       <c r="N156" s="9"/>
       <c r="O156" s="9"/>
-      <c r="P156" s="27"/>
-      <c r="Q156" s="28"/>
+      <c r="P156" s="29"/>
+      <c r="Q156" s="30"/>
     </row>
     <row r="157" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A157" s="5"/>
@@ -4435,12 +4720,12 @@
       <c r="H157" s="8"/>
       <c r="I157" s="9"/>
       <c r="J157" s="9"/>
-      <c r="K157" s="27"/>
-      <c r="L157" s="28"/>
+      <c r="K157" s="29"/>
+      <c r="L157" s="30"/>
       <c r="N157" s="9"/>
       <c r="O157" s="9"/>
-      <c r="P157" s="27"/>
-      <c r="Q157" s="28"/>
+      <c r="P157" s="29"/>
+      <c r="Q157" s="30"/>
     </row>
     <row r="158" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A158" s="5"/>
@@ -4453,12 +4738,12 @@
       <c r="H158" s="8"/>
       <c r="I158" s="9"/>
       <c r="J158" s="9"/>
-      <c r="K158" s="27"/>
-      <c r="L158" s="28"/>
+      <c r="K158" s="29"/>
+      <c r="L158" s="30"/>
       <c r="N158" s="9"/>
       <c r="O158" s="9"/>
-      <c r="P158" s="27"/>
-      <c r="Q158" s="28"/>
+      <c r="P158" s="29"/>
+      <c r="Q158" s="30"/>
     </row>
     <row r="159" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A159" s="5"/>
@@ -4471,8 +4756,8 @@
       <c r="H159" s="8"/>
       <c r="I159" s="9"/>
       <c r="J159" s="9"/>
-      <c r="K159" s="27"/>
-      <c r="L159" s="28"/>
+      <c r="K159" s="29"/>
+      <c r="L159" s="30"/>
       <c r="N159" s="9"/>
       <c r="O159" s="9"/>
       <c r="P159" s="6"/>
@@ -4507,8 +4792,8 @@
       <c r="K161" s="6"/>
       <c r="N161" s="9"/>
       <c r="O161" s="9"/>
-      <c r="P161" s="27"/>
-      <c r="Q161" s="28"/>
+      <c r="P161" s="29"/>
+      <c r="Q161" s="30"/>
     </row>
     <row r="162" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A162" s="5"/>
@@ -4521,12 +4806,12 @@
       <c r="H162" s="8"/>
       <c r="I162" s="9"/>
       <c r="J162" s="9"/>
-      <c r="K162" s="27"/>
-      <c r="L162" s="28"/>
+      <c r="K162" s="29"/>
+      <c r="L162" s="30"/>
       <c r="N162" s="9"/>
       <c r="O162" s="9"/>
-      <c r="P162" s="27"/>
-      <c r="Q162" s="28"/>
+      <c r="P162" s="29"/>
+      <c r="Q162" s="30"/>
     </row>
     <row r="163" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A163" s="5"/>
@@ -4539,12 +4824,12 @@
       <c r="H163" s="8"/>
       <c r="I163" s="9"/>
       <c r="J163" s="9"/>
-      <c r="K163" s="27"/>
-      <c r="L163" s="28"/>
+      <c r="K163" s="29"/>
+      <c r="L163" s="30"/>
       <c r="N163" s="9"/>
       <c r="O163" s="9"/>
-      <c r="P163" s="27"/>
-      <c r="Q163" s="28"/>
+      <c r="P163" s="29"/>
+      <c r="Q163" s="30"/>
     </row>
     <row r="164" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A164" s="5"/>
@@ -4557,12 +4842,12 @@
       <c r="H164" s="8"/>
       <c r="I164" s="9"/>
       <c r="J164" s="9"/>
-      <c r="K164" s="27"/>
-      <c r="L164" s="28"/>
+      <c r="K164" s="29"/>
+      <c r="L164" s="30"/>
       <c r="N164" s="9"/>
       <c r="O164" s="9"/>
-      <c r="P164" s="27"/>
-      <c r="Q164" s="28"/>
+      <c r="P164" s="29"/>
+      <c r="Q164" s="30"/>
     </row>
     <row r="165" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A165" s="5"/>
@@ -4575,8 +4860,8 @@
       <c r="H165" s="8"/>
       <c r="I165" s="9"/>
       <c r="J165" s="9"/>
-      <c r="K165" s="27"/>
-      <c r="L165" s="28"/>
+      <c r="K165" s="29"/>
+      <c r="L165" s="30"/>
       <c r="N165" s="9"/>
       <c r="O165" s="9"/>
       <c r="P165" s="6"/>
@@ -4611,8 +4896,8 @@
       <c r="K167" s="6"/>
       <c r="N167" s="9"/>
       <c r="O167" s="9"/>
-      <c r="P167" s="27"/>
-      <c r="Q167" s="28"/>
+      <c r="P167" s="29"/>
+      <c r="Q167" s="30"/>
     </row>
     <row r="168" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A168" s="5"/>
@@ -4625,12 +4910,12 @@
       <c r="H168" s="8"/>
       <c r="I168" s="9"/>
       <c r="J168" s="9"/>
-      <c r="K168" s="27"/>
-      <c r="L168" s="28"/>
+      <c r="K168" s="29"/>
+      <c r="L168" s="30"/>
       <c r="N168" s="9"/>
       <c r="O168" s="9"/>
-      <c r="P168" s="27"/>
-      <c r="Q168" s="28"/>
+      <c r="P168" s="29"/>
+      <c r="Q168" s="30"/>
     </row>
     <row r="169" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A169" s="5"/>
@@ -4643,12 +4928,12 @@
       <c r="H169" s="8"/>
       <c r="I169" s="9"/>
       <c r="J169" s="9"/>
-      <c r="K169" s="27"/>
-      <c r="L169" s="28"/>
+      <c r="K169" s="29"/>
+      <c r="L169" s="30"/>
       <c r="N169" s="9"/>
       <c r="O169" s="9"/>
-      <c r="P169" s="27"/>
-      <c r="Q169" s="28"/>
+      <c r="P169" s="29"/>
+      <c r="Q169" s="30"/>
     </row>
     <row r="170" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A170" s="5"/>
@@ -4661,12 +4946,12 @@
       <c r="H170" s="8"/>
       <c r="I170" s="9"/>
       <c r="J170" s="9"/>
-      <c r="K170" s="27"/>
-      <c r="L170" s="28"/>
+      <c r="K170" s="29"/>
+      <c r="L170" s="30"/>
       <c r="N170" s="9"/>
       <c r="O170" s="9"/>
-      <c r="P170" s="27"/>
-      <c r="Q170" s="28"/>
+      <c r="P170" s="29"/>
+      <c r="Q170" s="30"/>
     </row>
     <row r="171" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A171" s="5"/>
@@ -4679,8 +4964,8 @@
       <c r="H171" s="8"/>
       <c r="I171" s="9"/>
       <c r="J171" s="9"/>
-      <c r="K171" s="27"/>
-      <c r="L171" s="28"/>
+      <c r="K171" s="29"/>
+      <c r="L171" s="30"/>
       <c r="N171" s="9"/>
       <c r="O171" s="9"/>
       <c r="P171" s="6"/>
@@ -4715,8 +5000,8 @@
       <c r="K173" s="6"/>
       <c r="N173" s="9"/>
       <c r="O173" s="9"/>
-      <c r="P173" s="27"/>
-      <c r="Q173" s="28"/>
+      <c r="P173" s="29"/>
+      <c r="Q173" s="30"/>
     </row>
     <row r="174" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A174" s="5"/>
@@ -4729,12 +5014,12 @@
       <c r="H174" s="8"/>
       <c r="I174" s="9"/>
       <c r="J174" s="9"/>
-      <c r="K174" s="27"/>
-      <c r="L174" s="28"/>
+      <c r="K174" s="29"/>
+      <c r="L174" s="30"/>
       <c r="N174" s="9"/>
       <c r="O174" s="9"/>
-      <c r="P174" s="27"/>
-      <c r="Q174" s="28"/>
+      <c r="P174" s="29"/>
+      <c r="Q174" s="30"/>
     </row>
     <row r="175" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A175" s="5"/>
@@ -4747,12 +5032,12 @@
       <c r="H175" s="8"/>
       <c r="I175" s="9"/>
       <c r="J175" s="9"/>
-      <c r="K175" s="27"/>
-      <c r="L175" s="28"/>
+      <c r="K175" s="29"/>
+      <c r="L175" s="30"/>
       <c r="N175" s="9"/>
       <c r="O175" s="9"/>
-      <c r="P175" s="27"/>
-      <c r="Q175" s="28"/>
+      <c r="P175" s="29"/>
+      <c r="Q175" s="30"/>
     </row>
     <row r="176" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A176" s="5"/>
@@ -4765,12 +5050,12 @@
       <c r="H176" s="8"/>
       <c r="I176" s="9"/>
       <c r="J176" s="9"/>
-      <c r="K176" s="27"/>
-      <c r="L176" s="28"/>
+      <c r="K176" s="29"/>
+      <c r="L176" s="30"/>
       <c r="N176" s="9"/>
       <c r="O176" s="9"/>
-      <c r="P176" s="27"/>
-      <c r="Q176" s="28"/>
+      <c r="P176" s="29"/>
+      <c r="Q176" s="30"/>
     </row>
     <row r="177" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A177" s="5"/>
@@ -4783,8 +5068,8 @@
       <c r="H177" s="8"/>
       <c r="I177" s="9"/>
       <c r="J177" s="9"/>
-      <c r="K177" s="27"/>
-      <c r="L177" s="28"/>
+      <c r="K177" s="29"/>
+      <c r="L177" s="30"/>
       <c r="N177" s="9"/>
       <c r="O177" s="9"/>
       <c r="P177" s="6"/>
@@ -4819,8 +5104,8 @@
       <c r="K179" s="6"/>
       <c r="N179" s="9"/>
       <c r="O179" s="9"/>
-      <c r="P179" s="27"/>
-      <c r="Q179" s="28"/>
+      <c r="P179" s="29"/>
+      <c r="Q179" s="30"/>
     </row>
     <row r="180" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A180" s="5"/>
@@ -4833,12 +5118,12 @@
       <c r="H180" s="8"/>
       <c r="I180" s="9"/>
       <c r="J180" s="9"/>
-      <c r="K180" s="27"/>
-      <c r="L180" s="28"/>
+      <c r="K180" s="29"/>
+      <c r="L180" s="30"/>
       <c r="N180" s="9"/>
       <c r="O180" s="9"/>
-      <c r="P180" s="27"/>
-      <c r="Q180" s="28"/>
+      <c r="P180" s="29"/>
+      <c r="Q180" s="30"/>
     </row>
     <row r="181" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A181" s="5"/>
@@ -4851,12 +5136,12 @@
       <c r="H181" s="8"/>
       <c r="I181" s="9"/>
       <c r="J181" s="9"/>
-      <c r="K181" s="27"/>
-      <c r="L181" s="28"/>
+      <c r="K181" s="29"/>
+      <c r="L181" s="30"/>
       <c r="N181" s="9"/>
       <c r="O181" s="9"/>
-      <c r="P181" s="27"/>
-      <c r="Q181" s="28"/>
+      <c r="P181" s="29"/>
+      <c r="Q181" s="30"/>
     </row>
     <row r="182" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A182" s="5"/>
@@ -4869,12 +5154,12 @@
       <c r="H182" s="8"/>
       <c r="I182" s="9"/>
       <c r="J182" s="9"/>
-      <c r="K182" s="27"/>
-      <c r="L182" s="28"/>
+      <c r="K182" s="29"/>
+      <c r="L182" s="30"/>
       <c r="N182" s="9"/>
       <c r="O182" s="9"/>
-      <c r="P182" s="27"/>
-      <c r="Q182" s="28"/>
+      <c r="P182" s="29"/>
+      <c r="Q182" s="30"/>
     </row>
     <row r="183" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A183" s="5"/>
@@ -4887,8 +5172,8 @@
       <c r="H183" s="8"/>
       <c r="I183" s="9"/>
       <c r="J183" s="9"/>
-      <c r="K183" s="27"/>
-      <c r="L183" s="28"/>
+      <c r="K183" s="29"/>
+      <c r="L183" s="30"/>
       <c r="N183" s="9"/>
       <c r="O183" s="9"/>
       <c r="P183" s="6"/>
@@ -4923,8 +5208,8 @@
       <c r="K185" s="6"/>
       <c r="N185" s="9"/>
       <c r="O185" s="9"/>
-      <c r="P185" s="27"/>
-      <c r="Q185" s="28"/>
+      <c r="P185" s="29"/>
+      <c r="Q185" s="30"/>
     </row>
     <row r="186" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A186" s="5"/>
@@ -4937,12 +5222,12 @@
       <c r="H186" s="8"/>
       <c r="I186" s="9"/>
       <c r="J186" s="9"/>
-      <c r="K186" s="27"/>
-      <c r="L186" s="28"/>
+      <c r="K186" s="29"/>
+      <c r="L186" s="30"/>
       <c r="N186" s="9"/>
       <c r="O186" s="9"/>
-      <c r="P186" s="27"/>
-      <c r="Q186" s="28"/>
+      <c r="P186" s="29"/>
+      <c r="Q186" s="30"/>
     </row>
     <row r="187" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A187" s="5"/>
@@ -4955,12 +5240,12 @@
       <c r="H187" s="8"/>
       <c r="I187" s="9"/>
       <c r="J187" s="9"/>
-      <c r="K187" s="27"/>
-      <c r="L187" s="28"/>
+      <c r="K187" s="29"/>
+      <c r="L187" s="30"/>
       <c r="N187" s="9"/>
       <c r="O187" s="9"/>
-      <c r="P187" s="27"/>
-      <c r="Q187" s="28"/>
+      <c r="P187" s="29"/>
+      <c r="Q187" s="30"/>
     </row>
     <row r="188" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E188" s="16"/>
@@ -9865,40 +10150,190 @@
       <c r="H1004" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="251">
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K43:L43"/>
+  <mergeCells count="221">
+    <mergeCell ref="K94:L94"/>
+    <mergeCell ref="K95:L95"/>
+    <mergeCell ref="K96:L96"/>
+    <mergeCell ref="K99:L99"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="K101:L101"/>
+    <mergeCell ref="K102:L102"/>
+    <mergeCell ref="K103:L103"/>
+    <mergeCell ref="K104:L104"/>
+    <mergeCell ref="K83:L83"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="K86:L86"/>
+    <mergeCell ref="K87:L87"/>
+    <mergeCell ref="K88:L88"/>
+    <mergeCell ref="K91:L91"/>
+    <mergeCell ref="K92:L92"/>
+    <mergeCell ref="K93:L93"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="K78:L78"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="K168:L168"/>
+    <mergeCell ref="K180:L180"/>
+    <mergeCell ref="K181:L181"/>
+    <mergeCell ref="K182:L182"/>
+    <mergeCell ref="K183:L183"/>
+    <mergeCell ref="K186:L186"/>
+    <mergeCell ref="K187:L187"/>
+    <mergeCell ref="K169:L169"/>
+    <mergeCell ref="K170:L170"/>
+    <mergeCell ref="K171:L171"/>
+    <mergeCell ref="K174:L174"/>
+    <mergeCell ref="K175:L175"/>
+    <mergeCell ref="K176:L176"/>
+    <mergeCell ref="K177:L177"/>
+    <mergeCell ref="K153:L153"/>
+    <mergeCell ref="K154:L154"/>
+    <mergeCell ref="K157:L157"/>
+    <mergeCell ref="K158:L158"/>
+    <mergeCell ref="K159:L159"/>
+    <mergeCell ref="K162:L162"/>
+    <mergeCell ref="K163:L163"/>
+    <mergeCell ref="K164:L164"/>
+    <mergeCell ref="K165:L165"/>
+    <mergeCell ref="K136:L136"/>
+    <mergeCell ref="K137:L137"/>
+    <mergeCell ref="K138:L138"/>
+    <mergeCell ref="K141:L141"/>
+    <mergeCell ref="K142:L142"/>
+    <mergeCell ref="K145:L145"/>
+    <mergeCell ref="K146:L146"/>
+    <mergeCell ref="K149:L149"/>
+    <mergeCell ref="K150:L150"/>
+    <mergeCell ref="K127:L127"/>
+    <mergeCell ref="K128:L128"/>
+    <mergeCell ref="K129:L129"/>
+    <mergeCell ref="K130:L130"/>
+    <mergeCell ref="K131:L131"/>
+    <mergeCell ref="K132:L132"/>
+    <mergeCell ref="K133:L133"/>
+    <mergeCell ref="K134:L134"/>
+    <mergeCell ref="K135:L135"/>
+    <mergeCell ref="K116:L116"/>
+    <mergeCell ref="K117:L117"/>
+    <mergeCell ref="K118:L118"/>
+    <mergeCell ref="K119:L119"/>
+    <mergeCell ref="K120:L120"/>
+    <mergeCell ref="K121:L121"/>
+    <mergeCell ref="K122:L122"/>
+    <mergeCell ref="K125:L125"/>
+    <mergeCell ref="K126:L126"/>
+    <mergeCell ref="P107:Q107"/>
+    <mergeCell ref="K109:L109"/>
+    <mergeCell ref="K110:L110"/>
+    <mergeCell ref="K111:L111"/>
+    <mergeCell ref="K112:L112"/>
+    <mergeCell ref="K115:L115"/>
+    <mergeCell ref="K105:L105"/>
+    <mergeCell ref="K106:L106"/>
+    <mergeCell ref="K107:L107"/>
+    <mergeCell ref="K108:L108"/>
+    <mergeCell ref="P108:Q108"/>
+    <mergeCell ref="P109:Q109"/>
+    <mergeCell ref="P110:Q110"/>
+    <mergeCell ref="P111:Q111"/>
+    <mergeCell ref="P114:Q114"/>
+    <mergeCell ref="P115:Q115"/>
+    <mergeCell ref="P98:Q98"/>
+    <mergeCell ref="P99:Q99"/>
+    <mergeCell ref="P100:Q100"/>
+    <mergeCell ref="P101:Q101"/>
+    <mergeCell ref="P102:Q102"/>
+    <mergeCell ref="P103:Q103"/>
+    <mergeCell ref="P104:Q104"/>
+    <mergeCell ref="P105:Q105"/>
+    <mergeCell ref="P106:Q106"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P90:Q90"/>
+    <mergeCell ref="P91:Q91"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="P93:Q93"/>
+    <mergeCell ref="P94:Q94"/>
+    <mergeCell ref="P95:Q95"/>
+    <mergeCell ref="P70:Q70"/>
+    <mergeCell ref="P71:Q71"/>
+    <mergeCell ref="P72:Q72"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="P77:Q77"/>
+    <mergeCell ref="P82:Q82"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="P84:Q84"/>
+    <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="P63:Q63"/>
+    <mergeCell ref="P64:Q64"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="P182:Q182"/>
+    <mergeCell ref="P185:Q185"/>
+    <mergeCell ref="P186:Q186"/>
+    <mergeCell ref="P187:Q187"/>
+    <mergeCell ref="P168:Q168"/>
+    <mergeCell ref="P169:Q169"/>
+    <mergeCell ref="P170:Q170"/>
+    <mergeCell ref="P173:Q173"/>
+    <mergeCell ref="P174:Q174"/>
+    <mergeCell ref="P175:Q175"/>
+    <mergeCell ref="P176:Q176"/>
+    <mergeCell ref="P158:Q158"/>
+    <mergeCell ref="P161:Q161"/>
+    <mergeCell ref="P162:Q162"/>
+    <mergeCell ref="P163:Q163"/>
+    <mergeCell ref="P164:Q164"/>
+    <mergeCell ref="P167:Q167"/>
+    <mergeCell ref="P179:Q179"/>
+    <mergeCell ref="P180:Q180"/>
+    <mergeCell ref="P181:Q181"/>
+    <mergeCell ref="P141:Q141"/>
+    <mergeCell ref="P144:Q144"/>
+    <mergeCell ref="P145:Q145"/>
+    <mergeCell ref="P148:Q148"/>
+    <mergeCell ref="P149:Q149"/>
+    <mergeCell ref="P152:Q152"/>
+    <mergeCell ref="P153:Q153"/>
+    <mergeCell ref="P156:Q156"/>
+    <mergeCell ref="P157:Q157"/>
+    <mergeCell ref="P130:Q130"/>
+    <mergeCell ref="P131:Q131"/>
+    <mergeCell ref="P132:Q132"/>
+    <mergeCell ref="P133:Q133"/>
+    <mergeCell ref="P134:Q134"/>
+    <mergeCell ref="P135:Q135"/>
+    <mergeCell ref="P136:Q136"/>
+    <mergeCell ref="P137:Q137"/>
+    <mergeCell ref="P140:Q140"/>
+    <mergeCell ref="P119:Q119"/>
+    <mergeCell ref="P120:Q120"/>
+    <mergeCell ref="P121:Q121"/>
+    <mergeCell ref="P124:Q124"/>
+    <mergeCell ref="P125:Q125"/>
+    <mergeCell ref="P126:Q126"/>
+    <mergeCell ref="P127:Q127"/>
+    <mergeCell ref="P128:Q128"/>
+    <mergeCell ref="P129:Q129"/>
     <mergeCell ref="P116:Q116"/>
     <mergeCell ref="P117:Q117"/>
     <mergeCell ref="P118:Q118"/>
@@ -9923,200 +10358,20 @@
     <mergeCell ref="P56:Q56"/>
     <mergeCell ref="P57:Q57"/>
     <mergeCell ref="P60:Q60"/>
-    <mergeCell ref="P119:Q119"/>
-    <mergeCell ref="P120:Q120"/>
-    <mergeCell ref="P121:Q121"/>
-    <mergeCell ref="P124:Q124"/>
-    <mergeCell ref="P125:Q125"/>
-    <mergeCell ref="P126:Q126"/>
-    <mergeCell ref="P127:Q127"/>
-    <mergeCell ref="P128:Q128"/>
-    <mergeCell ref="P129:Q129"/>
-    <mergeCell ref="P130:Q130"/>
-    <mergeCell ref="P131:Q131"/>
-    <mergeCell ref="P132:Q132"/>
-    <mergeCell ref="P133:Q133"/>
-    <mergeCell ref="P134:Q134"/>
-    <mergeCell ref="P135:Q135"/>
-    <mergeCell ref="P136:Q136"/>
-    <mergeCell ref="P137:Q137"/>
-    <mergeCell ref="P140:Q140"/>
-    <mergeCell ref="P141:Q141"/>
-    <mergeCell ref="P144:Q144"/>
-    <mergeCell ref="P145:Q145"/>
-    <mergeCell ref="P148:Q148"/>
-    <mergeCell ref="P149:Q149"/>
-    <mergeCell ref="P152:Q152"/>
-    <mergeCell ref="P153:Q153"/>
-    <mergeCell ref="P156:Q156"/>
-    <mergeCell ref="P157:Q157"/>
-    <mergeCell ref="P158:Q158"/>
-    <mergeCell ref="P161:Q161"/>
-    <mergeCell ref="P162:Q162"/>
-    <mergeCell ref="P163:Q163"/>
-    <mergeCell ref="P164:Q164"/>
-    <mergeCell ref="P167:Q167"/>
-    <mergeCell ref="P179:Q179"/>
-    <mergeCell ref="P180:Q180"/>
-    <mergeCell ref="P181:Q181"/>
-    <mergeCell ref="P182:Q182"/>
-    <mergeCell ref="P185:Q185"/>
-    <mergeCell ref="P186:Q186"/>
-    <mergeCell ref="P187:Q187"/>
-    <mergeCell ref="P168:Q168"/>
-    <mergeCell ref="P169:Q169"/>
-    <mergeCell ref="P170:Q170"/>
-    <mergeCell ref="P173:Q173"/>
-    <mergeCell ref="P174:Q174"/>
-    <mergeCell ref="P175:Q175"/>
-    <mergeCell ref="P176:Q176"/>
-    <mergeCell ref="P61:Q61"/>
-    <mergeCell ref="P62:Q62"/>
-    <mergeCell ref="P63:Q63"/>
-    <mergeCell ref="P64:Q64"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="P66:Q66"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P69:Q69"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="P71:Q71"/>
-    <mergeCell ref="P72:Q72"/>
-    <mergeCell ref="P73:Q73"/>
-    <mergeCell ref="P76:Q76"/>
-    <mergeCell ref="P77:Q77"/>
-    <mergeCell ref="P82:Q82"/>
-    <mergeCell ref="P83:Q83"/>
-    <mergeCell ref="P84:Q84"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P90:Q90"/>
-    <mergeCell ref="P91:Q91"/>
-    <mergeCell ref="P92:Q92"/>
-    <mergeCell ref="P93:Q93"/>
-    <mergeCell ref="P94:Q94"/>
-    <mergeCell ref="P95:Q95"/>
-    <mergeCell ref="P98:Q98"/>
-    <mergeCell ref="P99:Q99"/>
-    <mergeCell ref="P100:Q100"/>
-    <mergeCell ref="P101:Q101"/>
-    <mergeCell ref="P102:Q102"/>
-    <mergeCell ref="P103:Q103"/>
-    <mergeCell ref="P104:Q104"/>
-    <mergeCell ref="P105:Q105"/>
-    <mergeCell ref="P106:Q106"/>
-    <mergeCell ref="P107:Q107"/>
-    <mergeCell ref="K109:L109"/>
-    <mergeCell ref="K110:L110"/>
-    <mergeCell ref="K111:L111"/>
-    <mergeCell ref="K112:L112"/>
-    <mergeCell ref="K115:L115"/>
-    <mergeCell ref="K105:L105"/>
-    <mergeCell ref="K106:L106"/>
-    <mergeCell ref="K107:L107"/>
-    <mergeCell ref="K108:L108"/>
-    <mergeCell ref="P108:Q108"/>
-    <mergeCell ref="P109:Q109"/>
-    <mergeCell ref="P110:Q110"/>
-    <mergeCell ref="P111:Q111"/>
-    <mergeCell ref="P114:Q114"/>
-    <mergeCell ref="P115:Q115"/>
-    <mergeCell ref="K116:L116"/>
-    <mergeCell ref="K117:L117"/>
-    <mergeCell ref="K118:L118"/>
-    <mergeCell ref="K119:L119"/>
-    <mergeCell ref="K120:L120"/>
-    <mergeCell ref="K121:L121"/>
-    <mergeCell ref="K122:L122"/>
-    <mergeCell ref="K125:L125"/>
-    <mergeCell ref="K126:L126"/>
-    <mergeCell ref="K127:L127"/>
-    <mergeCell ref="K128:L128"/>
-    <mergeCell ref="K129:L129"/>
-    <mergeCell ref="K130:L130"/>
-    <mergeCell ref="K131:L131"/>
-    <mergeCell ref="K132:L132"/>
-    <mergeCell ref="K133:L133"/>
-    <mergeCell ref="K134:L134"/>
-    <mergeCell ref="K135:L135"/>
-    <mergeCell ref="K136:L136"/>
-    <mergeCell ref="K137:L137"/>
-    <mergeCell ref="K138:L138"/>
-    <mergeCell ref="K141:L141"/>
-    <mergeCell ref="K142:L142"/>
-    <mergeCell ref="K145:L145"/>
-    <mergeCell ref="K146:L146"/>
-    <mergeCell ref="K149:L149"/>
-    <mergeCell ref="K150:L150"/>
-    <mergeCell ref="K153:L153"/>
-    <mergeCell ref="K154:L154"/>
-    <mergeCell ref="K157:L157"/>
-    <mergeCell ref="K158:L158"/>
-    <mergeCell ref="K159:L159"/>
-    <mergeCell ref="K162:L162"/>
-    <mergeCell ref="K163:L163"/>
-    <mergeCell ref="K164:L164"/>
-    <mergeCell ref="K165:L165"/>
-    <mergeCell ref="K168:L168"/>
-    <mergeCell ref="K180:L180"/>
-    <mergeCell ref="K181:L181"/>
-    <mergeCell ref="K182:L182"/>
-    <mergeCell ref="K183:L183"/>
-    <mergeCell ref="K186:L186"/>
-    <mergeCell ref="K187:L187"/>
-    <mergeCell ref="K169:L169"/>
-    <mergeCell ref="K170:L170"/>
-    <mergeCell ref="K171:L171"/>
-    <mergeCell ref="K174:L174"/>
-    <mergeCell ref="K175:L175"/>
-    <mergeCell ref="K176:L176"/>
-    <mergeCell ref="K177:L177"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="K77:L77"/>
-    <mergeCell ref="K78:L78"/>
-    <mergeCell ref="K83:L83"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="K86:L86"/>
-    <mergeCell ref="K87:L87"/>
-    <mergeCell ref="K88:L88"/>
-    <mergeCell ref="K91:L91"/>
-    <mergeCell ref="K92:L92"/>
-    <mergeCell ref="K93:L93"/>
-    <mergeCell ref="K94:L94"/>
-    <mergeCell ref="K95:L95"/>
-    <mergeCell ref="K96:L96"/>
-    <mergeCell ref="K99:L99"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="K101:L101"/>
-    <mergeCell ref="K102:L102"/>
-    <mergeCell ref="K103:L103"/>
-    <mergeCell ref="K104:L104"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>